<commit_message>
working on driver again
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjferrante/Desktop/afs-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E4749-B305-AC4F-9CC3-B7FA2C8A284F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD1305C-EFA6-AE4B-8E88-43965EE1146A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A7FC1753-936A-E24E-9776-AF2CB855BB60}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A7FC1753-936A-E24E-9776-AF2CB855BB60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="1301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="1301">
   <si>
     <t>Exercise Name</t>
   </si>
@@ -4323,8 +4323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E02BC4-7A5F-4A44-99BE-655C181A9DA1}">
   <dimension ref="A1:J1303"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4358,7 +4358,9 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="J1" s="1" t="s">
         <v>908</v>
       </c>
@@ -10900,7 +10902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252555A8-30F1-8B44-9E37-D2B34DB1D871}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>